<commit_message>
Updated Excel Sheet Connections
</commit_message>
<xml_diff>
--- a/Engine CAD/APL TCA Dimensions.xlsx
+++ b/Engine CAD/APL TCA Dimensions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\UC DAVIS\APL\Engine CAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuval\Documents\GitHub\Mu-Engine\Engine CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56AB256-6060-49EE-8DC2-507ABD3E40B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D4FB84-9E0D-4973-BAE9-64F4DEF3C352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="480" windowWidth="25580" windowHeight="15260" xr2:uid="{A9254718-37E5-4F3C-B873-A41725991B0A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12980" windowHeight="15280" xr2:uid="{A9254718-37E5-4F3C-B873-A41725991B0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>Screwing Space Section</t>
   </si>
@@ -199,9 +199,6 @@
   </si>
   <si>
     <t>Throat Curve Radius/Nozzle Throat Radius</t>
-  </si>
-  <si>
-    <t>(4.5/2)-0.15</t>
   </si>
 </sst>
 </file>
@@ -588,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C6B68B-2FCF-4A43-9246-EB6A4ACF616D}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -970,9 +967,7 @@
         <f>(4.5/2)-0.15</f>
         <v>2.1</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="D45" s="5"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">

</xml_diff>